<commit_message>
fix test case 1 + test case 2
</commit_message>
<xml_diff>
--- a/documents/8.1.ProjectTestCaseSprint1.xlsx
+++ b/documents/8.1.ProjectTestCaseSprint1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E24B45-ADBC-4864-A60C-74C3A94884FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2F822-1789-460D-8E44-0B9074DCE748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="576" windowWidth="23256" windowHeight="13176" tabRatio="896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="896" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trường hợp kiểm thử" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="1026">
   <si>
     <t>TEST CASE SYSTEM SPRINT 1</t>
   </si>
@@ -3527,13 +3527,31 @@
     <t>1 . Dừng video 2 Mở ở tab ghi chú 3 Ghi chú</t>
   </si>
   <si>
-    <t>Ghi chú ngay thười điểm dừng video</t>
-  </si>
-  <si>
     <t>Ghi chú không hiện</t>
   </si>
   <si>
     <t>Đang phát triển</t>
+  </si>
+  <si>
+    <t>Hệ thống không hiển thị thông báo lỗi "Mật khẩu là bắt buộc".</t>
+  </si>
+  <si>
+    <t>Hệ thống không hiển thị thông báo lỗi "Tên đầy đủ là bắt buộc".</t>
+  </si>
+  <si>
+    <t>Hệ thống không hiển thị thông báo lỗi "Mật khẩu và xác nhận mật khẩu không khớp".</t>
+  </si>
+  <si>
+    <t>Hệ thống không hiển thị thông báo lỗi "Mật khẩu phải có ít nhất một ký tự đặc biệt và một chữ hoa".</t>
+  </si>
+  <si>
+    <t>Hệ thống không hiển thị thông báo lỗi "Mật khẩu phải có ít nhất 6 ký tự".</t>
+  </si>
+  <si>
+    <t>Không loading được</t>
+  </si>
+  <si>
+    <t>Ghi chú ngay thời điểm dừng video</t>
   </si>
 </sst>
 </file>
@@ -4961,6 +4979,42 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5012,12 +5066,33 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -5042,27 +5117,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -5140,42 +5194,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6229,7 +6247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C19" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
@@ -6243,31 +6261,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="196"/>
+      <c r="B1" s="207"/>
+      <c r="C1" s="207"/>
+      <c r="D1" s="207"/>
+      <c r="E1" s="208"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="197"/>
-      <c r="B2" s="198"/>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="199"/>
+      <c r="A2" s="209"/>
+      <c r="B2" s="210"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="211"/>
     </row>
     <row r="3" spans="1:5" ht="65.25" customHeight="1">
       <c r="A3" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="212" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="201"/>
-      <c r="D3" s="201"/>
-      <c r="E3" s="202"/>
+      <c r="C3" s="213"/>
+      <c r="D3" s="213"/>
+      <c r="E3" s="214"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="134" t="s">
@@ -6287,10 +6305,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A5" s="205">
+      <c r="A5" s="217">
         <v>1</v>
       </c>
-      <c r="B5" s="191" t="s">
+      <c r="B5" s="203" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="132" t="s">
@@ -6302,8 +6320,8 @@
       <c r="E5" s="93"/>
     </row>
     <row r="6" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A6" s="205"/>
-      <c r="B6" s="191"/>
+      <c r="A6" s="217"/>
+      <c r="B6" s="203"/>
       <c r="C6" s="65" t="s">
         <v>10</v>
       </c>
@@ -6313,8 +6331,8 @@
       <c r="E6" s="93"/>
     </row>
     <row r="7" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A7" s="205"/>
-      <c r="B7" s="191"/>
+      <c r="A7" s="217"/>
+      <c r="B7" s="203"/>
       <c r="C7" s="132" t="s">
         <v>11</v>
       </c>
@@ -6324,10 +6342,10 @@
       <c r="E7" s="93"/>
     </row>
     <row r="8" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A8" s="192">
+      <c r="A8" s="204">
         <v>2</v>
       </c>
-      <c r="B8" s="203" t="s">
+      <c r="B8" s="215" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="132" t="s">
@@ -6339,8 +6357,8 @@
       <c r="E8" s="93"/>
     </row>
     <row r="9" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A9" s="207"/>
-      <c r="B9" s="206"/>
+      <c r="A9" s="219"/>
+      <c r="B9" s="218"/>
       <c r="C9" s="132" t="s">
         <v>14</v>
       </c>
@@ -6350,8 +6368,8 @@
       <c r="E9" s="93"/>
     </row>
     <row r="10" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A10" s="193"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="205"/>
+      <c r="B10" s="216"/>
       <c r="C10" s="132" t="s">
         <v>15</v>
       </c>
@@ -6361,10 +6379,10 @@
       <c r="E10" s="93"/>
     </row>
     <row r="11" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A11" s="205">
+      <c r="A11" s="217">
         <v>3</v>
       </c>
-      <c r="B11" s="203" t="s">
+      <c r="B11" s="215" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="132" t="s">
@@ -6376,8 +6394,8 @@
       <c r="E11" s="93"/>
     </row>
     <row r="12" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A12" s="205"/>
-      <c r="B12" s="204"/>
+      <c r="A12" s="217"/>
+      <c r="B12" s="216"/>
       <c r="C12" s="132" t="s">
         <v>18</v>
       </c>
@@ -6387,10 +6405,10 @@
       <c r="E12" s="93"/>
     </row>
     <row r="13" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A13" s="192">
+      <c r="A13" s="204">
         <v>4</v>
       </c>
-      <c r="B13" s="191" t="s">
+      <c r="B13" s="203" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="132" t="s">
@@ -6402,8 +6420,8 @@
       <c r="E13" s="93"/>
     </row>
     <row r="14" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A14" s="193"/>
-      <c r="B14" s="191"/>
+      <c r="A14" s="205"/>
+      <c r="B14" s="203"/>
       <c r="C14" s="132" t="s">
         <v>21</v>
       </c>
@@ -6473,7 +6491,7 @@
   </sheetPr>
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G19" sqref="G19:G27"/>
     </sheetView>
   </sheetViews>
@@ -6500,13 +6518,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="246" t="s">
+      <c r="B1" s="258" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -6520,13 +6538,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -6635,68 +6653,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -6706,7 +6724,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -6716,25 +6734,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:15" s="41" customFormat="1">
-      <c r="A10" s="234" t="s">
+      <c r="A10" s="246" t="s">
         <v>612</v>
       </c>
-      <c r="B10" s="234"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="234"/>
-      <c r="H10" s="234"/>
-      <c r="I10" s="234"/>
-      <c r="J10" s="234"/>
-      <c r="K10" s="234"/>
-      <c r="L10" s="234"/>
-      <c r="M10" s="234"/>
-      <c r="N10" s="234"/>
+      <c r="B10" s="246"/>
+      <c r="C10" s="246"/>
+      <c r="D10" s="246"/>
+      <c r="E10" s="246"/>
+      <c r="F10" s="246"/>
+      <c r="G10" s="246"/>
+      <c r="H10" s="246"/>
+      <c r="I10" s="246"/>
+      <c r="J10" s="246"/>
+      <c r="K10" s="246"/>
+      <c r="L10" s="246"/>
+      <c r="M10" s="246"/>
+      <c r="N10" s="246"/>
       <c r="O10" s="76"/>
     </row>
     <row r="11" spans="1:15" s="42" customFormat="1" ht="72" customHeight="1">
@@ -7521,13 +7539,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="J7:J9"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -7536,6 +7547,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="J7:J9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="K19:K27 G19:G27 G11:G17 K11:K17" xr:uid="{C86AFFE1-8497-43E8-A278-02C6F231645D}">
@@ -7553,7 +7571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A84C2F-9FEE-4783-97F2-A9A216EBBC9F}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:G24"/>
     </sheetView>
   </sheetViews>
@@ -7580,13 +7598,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="232" t="s">
+      <c r="B1" s="244" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -7600,13 +7618,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -7717,68 +7735,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:15" s="29" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="29" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:15" s="29" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -7788,7 +7806,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -7798,25 +7816,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:15" s="29" customFormat="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="247" t="s">
         <v>688</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="247"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
       <c r="O10" s="73"/>
     </row>
     <row r="11" spans="1:15" s="38" customFormat="1" ht="72" customHeight="1">
@@ -8545,7 +8563,7 @@
   </sheetPr>
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:G37"/>
     </sheetView>
   </sheetViews>
@@ -8572,13 +8590,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -8592,13 +8610,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>751</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -8707,68 +8725,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -8778,7 +8796,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -8788,25 +8806,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:15" s="41" customFormat="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="247" t="s">
         <v>612</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="247"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
       <c r="O10" s="76"/>
     </row>
     <row r="11" spans="1:15" s="42" customFormat="1" ht="72" customHeight="1">
@@ -9963,7 +9981,7 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:G22"/>
     </sheetView>
   </sheetViews>
@@ -9990,13 +10008,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -10010,13 +10028,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>870</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -10125,68 +10143,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="41" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="41" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:14" s="41" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -10196,7 +10214,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -10206,25 +10224,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:14" s="41" customFormat="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="247" t="s">
         <v>871</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="247"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
     </row>
     <row r="11" spans="1:14" s="42" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="68" t="s">
@@ -10807,13 +10825,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="J7:J9"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -10822,6 +10833,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="J7:J9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="K15:K22 K11:K13 G11:G13 G15:G22" xr:uid="{22D30220-AAEB-45B6-94F3-36659780E18D}">
@@ -10842,7 +10860,7 @@
   </sheetPr>
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:G29"/>
     </sheetView>
   </sheetViews>
@@ -10869,13 +10887,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -10889,13 +10907,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -11002,68 +11020,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="29" customFormat="1">
-      <c r="A7" s="247" t="s">
+      <c r="A7" s="259" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="247" t="s">
+      <c r="B7" s="259" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="247" t="s">
+      <c r="C7" s="259" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="247" t="s">
+      <c r="D7" s="259" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="247" t="s">
+      <c r="E7" s="259" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="247" t="s">
+      <c r="F7" s="259" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="247" t="s">
+      <c r="G7" s="259" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="247"/>
-      <c r="I7" s="247"/>
-      <c r="J7" s="248" t="s">
+      <c r="H7" s="259"/>
+      <c r="I7" s="259"/>
+      <c r="J7" s="260" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="247" t="s">
+      <c r="K7" s="259" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="247"/>
-      <c r="M7" s="247"/>
-      <c r="N7" s="247" t="s">
+      <c r="L7" s="259"/>
+      <c r="M7" s="259"/>
+      <c r="N7" s="259" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="29" customFormat="1">
-      <c r="A8" s="247"/>
-      <c r="B8" s="247"/>
-      <c r="C8" s="247"/>
-      <c r="D8" s="247"/>
-      <c r="E8" s="247"/>
-      <c r="F8" s="247"/>
-      <c r="G8" s="247" t="s">
+      <c r="A8" s="259"/>
+      <c r="B8" s="259"/>
+      <c r="C8" s="259"/>
+      <c r="D8" s="259"/>
+      <c r="E8" s="259"/>
+      <c r="F8" s="259"/>
+      <c r="G8" s="259" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="247"/>
-      <c r="I8" s="247"/>
-      <c r="J8" s="249"/>
-      <c r="K8" s="247" t="s">
+      <c r="H8" s="259"/>
+      <c r="I8" s="259"/>
+      <c r="J8" s="261"/>
+      <c r="K8" s="259" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="247"/>
-      <c r="M8" s="247"/>
-      <c r="N8" s="247"/>
+      <c r="L8" s="259"/>
+      <c r="M8" s="259"/>
+      <c r="N8" s="259"/>
     </row>
     <row r="9" spans="1:14" s="29" customFormat="1">
-      <c r="A9" s="247"/>
-      <c r="B9" s="247"/>
-      <c r="C9" s="247"/>
-      <c r="D9" s="247"/>
-      <c r="E9" s="247"/>
-      <c r="F9" s="247"/>
+      <c r="A9" s="259"/>
+      <c r="B9" s="259"/>
+      <c r="C9" s="259"/>
+      <c r="D9" s="259"/>
+      <c r="E9" s="259"/>
+      <c r="F9" s="259"/>
       <c r="G9" s="175" t="s">
         <v>73</v>
       </c>
@@ -11073,7 +11091,7 @@
       <c r="I9" s="177" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="250"/>
+      <c r="J9" s="262"/>
       <c r="K9" s="175" t="s">
         <v>73</v>
       </c>
@@ -11083,25 +11101,25 @@
       <c r="M9" s="177" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="247"/>
+      <c r="N9" s="259"/>
     </row>
     <row r="10" spans="1:14" s="29" customFormat="1">
-      <c r="A10" s="234" t="s">
+      <c r="A10" s="246" t="s">
         <v>923</v>
       </c>
-      <c r="B10" s="234"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="234"/>
-      <c r="H10" s="234"/>
-      <c r="I10" s="234"/>
-      <c r="J10" s="234"/>
-      <c r="K10" s="234"/>
-      <c r="L10" s="234"/>
-      <c r="M10" s="234"/>
-      <c r="N10" s="234"/>
+      <c r="B10" s="246"/>
+      <c r="C10" s="246"/>
+      <c r="D10" s="246"/>
+      <c r="E10" s="246"/>
+      <c r="F10" s="246"/>
+      <c r="G10" s="246"/>
+      <c r="H10" s="246"/>
+      <c r="I10" s="246"/>
+      <c r="J10" s="246"/>
+      <c r="K10" s="246"/>
+      <c r="L10" s="246"/>
+      <c r="M10" s="246"/>
+      <c r="N10" s="246"/>
     </row>
     <row r="11" spans="1:14" s="38" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="68" t="s">
@@ -12103,24 +12121,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="25.5">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="235" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
-      <c r="K1" s="216"/>
-      <c r="L1" s="216"/>
-      <c r="M1" s="216"/>
-      <c r="N1" s="216"/>
-      <c r="O1" s="216"/>
-      <c r="P1" s="216"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="235"/>
+      <c r="D1" s="235"/>
+      <c r="E1" s="235"/>
+      <c r="F1" s="235"/>
+      <c r="G1" s="235"/>
+      <c r="H1" s="235"/>
+      <c r="I1" s="235"/>
+      <c r="J1" s="235"/>
+      <c r="K1" s="235"/>
+      <c r="L1" s="235"/>
+      <c r="M1" s="235"/>
+      <c r="N1" s="235"/>
+      <c r="O1" s="235"/>
+      <c r="P1" s="235"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="12.75">
       <c r="A2" s="2"/>
@@ -12144,22 +12162,22 @@
       <c r="A3" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="217" t="s">
+      <c r="B3" s="236" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="217"/>
+      <c r="C3" s="236"/>
       <c r="D3" s="167"/>
-      <c r="E3" s="209" t="s">
+      <c r="E3" s="223" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="209"/>
-      <c r="G3" s="209"/>
-      <c r="H3" s="210" t="s">
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="229" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="211"/>
-      <c r="J3" s="211"/>
-      <c r="K3" s="212"/>
+      <c r="I3" s="230"/>
+      <c r="J3" s="230"/>
+      <c r="K3" s="231"/>
       <c r="L3" s="136"/>
       <c r="M3" s="136"/>
       <c r="N3" s="136"/>
@@ -12168,20 +12186,20 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" ht="16.5">
       <c r="A4" s="135"/>
-      <c r="B4" s="208"/>
-      <c r="C4" s="208"/>
+      <c r="B4" s="222"/>
+      <c r="C4" s="222"/>
       <c r="D4" s="166"/>
-      <c r="E4" s="209" t="s">
+      <c r="E4" s="223" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="213" t="s">
+      <c r="F4" s="223"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="232" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="214"/>
-      <c r="J4" s="214"/>
-      <c r="K4" s="215"/>
+      <c r="I4" s="233"/>
+      <c r="J4" s="233"/>
+      <c r="K4" s="234"/>
       <c r="L4" s="166"/>
       <c r="M4" s="136"/>
       <c r="N4" s="136"/>
@@ -12190,20 +12208,20 @@
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="16.5">
       <c r="A5" s="135"/>
-      <c r="B5" s="208"/>
-      <c r="C5" s="208"/>
+      <c r="B5" s="222"/>
+      <c r="C5" s="222"/>
       <c r="D5" s="166"/>
-      <c r="E5" s="209" t="s">
+      <c r="E5" s="223" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="209"/>
-      <c r="G5" s="209"/>
-      <c r="H5" s="222">
+      <c r="F5" s="223"/>
+      <c r="G5" s="223"/>
+      <c r="H5" s="226">
         <v>44114</v>
       </c>
-      <c r="I5" s="223"/>
-      <c r="J5" s="223"/>
-      <c r="K5" s="224"/>
+      <c r="I5" s="227"/>
+      <c r="J5" s="227"/>
+      <c r="K5" s="228"/>
       <c r="L5" s="166"/>
       <c r="M5" s="136"/>
       <c r="N5" s="136"/>
@@ -12214,18 +12232,18 @@
       <c r="A6" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="220" t="s">
+      <c r="B6" s="224" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="220"/>
-      <c r="D6" s="220"/>
-      <c r="E6" s="220"/>
-      <c r="F6" s="220"/>
-      <c r="G6" s="220"/>
-      <c r="H6" s="220"/>
-      <c r="I6" s="220"/>
-      <c r="J6" s="220"/>
-      <c r="K6" s="220"/>
+      <c r="C6" s="224"/>
+      <c r="D6" s="224"/>
+      <c r="E6" s="224"/>
+      <c r="F6" s="224"/>
+      <c r="G6" s="224"/>
+      <c r="H6" s="224"/>
+      <c r="I6" s="224"/>
+      <c r="J6" s="224"/>
+      <c r="K6" s="224"/>
       <c r="L6" s="168"/>
       <c r="M6" s="138"/>
       <c r="N6" s="138"/>
@@ -12235,52 +12253,52 @@
     <row r="7" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1">
       <c r="A7" s="139"/>
       <c r="B7" s="140"/>
-      <c r="C7" s="221" t="s">
+      <c r="C7" s="225" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="221"/>
-      <c r="E7" s="221" t="s">
+      <c r="D7" s="225"/>
+      <c r="E7" s="225" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="221"/>
-      <c r="G7" s="221" t="s">
+      <c r="F7" s="225"/>
+      <c r="G7" s="225" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="221"/>
-      <c r="I7" s="221" t="s">
+      <c r="H7" s="225"/>
+      <c r="I7" s="225" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="221"/>
-      <c r="K7" s="221" t="s">
+      <c r="J7" s="225"/>
+      <c r="K7" s="225" t="s">
         <v>38</v>
       </c>
-      <c r="L7" s="221"/>
-      <c r="M7" s="218" t="s">
+      <c r="L7" s="225"/>
+      <c r="M7" s="220" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="218"/>
-      <c r="O7" s="219" t="s">
+      <c r="N7" s="220"/>
+      <c r="O7" s="221" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="219"/>
+      <c r="P7" s="221"/>
     </row>
     <row r="8" spans="1:16" s="1" customFormat="1" ht="16.5">
       <c r="A8" s="141"/>
       <c r="B8" s="142"/>
-      <c r="C8" s="221"/>
-      <c r="D8" s="221"/>
-      <c r="E8" s="221"/>
-      <c r="F8" s="221"/>
-      <c r="G8" s="221"/>
-      <c r="H8" s="221"/>
-      <c r="I8" s="221"/>
-      <c r="J8" s="221"/>
-      <c r="K8" s="221"/>
-      <c r="L8" s="221"/>
-      <c r="M8" s="218"/>
-      <c r="N8" s="218"/>
-      <c r="O8" s="219"/>
-      <c r="P8" s="219"/>
+      <c r="C8" s="225"/>
+      <c r="D8" s="225"/>
+      <c r="E8" s="225"/>
+      <c r="F8" s="225"/>
+      <c r="G8" s="225"/>
+      <c r="H8" s="225"/>
+      <c r="I8" s="225"/>
+      <c r="J8" s="225"/>
+      <c r="K8" s="225"/>
+      <c r="L8" s="225"/>
+      <c r="M8" s="220"/>
+      <c r="N8" s="220"/>
+      <c r="O8" s="221"/>
+      <c r="P8" s="221"/>
     </row>
     <row r="9" spans="1:16" s="5" customFormat="1" ht="22.5" customHeight="1">
       <c r="A9" s="143" t="s">
@@ -13001,6 +13019,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
     <mergeCell ref="M7:N8"/>
     <mergeCell ref="O7:P8"/>
     <mergeCell ref="B5:C5"/>
@@ -13012,13 +13037,6 @@
     <mergeCell ref="I7:J8"/>
     <mergeCell ref="K7:L8"/>
     <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -13032,8 +13050,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G29"/>
+    <sheetView topLeftCell="C19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -13059,13 +13077,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -13193,68 +13211,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="41" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="41" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:14" s="41" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="169" t="s">
         <v>73</v>
       </c>
@@ -13264,7 +13282,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="169" t="s">
         <v>73</v>
       </c>
@@ -13274,25 +13292,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:14" s="41" customFormat="1">
-      <c r="A10" s="227" t="s">
+      <c r="A10" s="239" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="227"/>
-      <c r="C10" s="227"/>
-      <c r="D10" s="227"/>
-      <c r="E10" s="227"/>
-      <c r="F10" s="227"/>
-      <c r="G10" s="227"/>
-      <c r="H10" s="227"/>
-      <c r="I10" s="227"/>
-      <c r="J10" s="227"/>
-      <c r="K10" s="227"/>
-      <c r="L10" s="227"/>
-      <c r="M10" s="227"/>
-      <c r="N10" s="227"/>
+      <c r="B10" s="239"/>
+      <c r="C10" s="239"/>
+      <c r="D10" s="239"/>
+      <c r="E10" s="239"/>
+      <c r="F10" s="239"/>
+      <c r="G10" s="239"/>
+      <c r="H10" s="239"/>
+      <c r="I10" s="239"/>
+      <c r="J10" s="239"/>
+      <c r="K10" s="239"/>
+      <c r="L10" s="239"/>
+      <c r="M10" s="239"/>
+      <c r="N10" s="239"/>
     </row>
     <row r="11" spans="1:14" s="42" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="68" t="s">
@@ -13631,10 +13649,10 @@
       <c r="N18" s="55"/>
     </row>
     <row r="19" spans="1:18" s="40" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A19" s="225" t="s">
+      <c r="A19" s="237" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="226"/>
+      <c r="B19" s="238"/>
       <c r="C19" s="97"/>
       <c r="D19" s="97"/>
       <c r="E19" s="97"/>
@@ -14253,8 +14271,8 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G32"/>
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -14280,13 +14298,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="237" t="s">
+      <c r="B1" s="249" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="237"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -14300,13 +14318,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -14415,68 +14433,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="29" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="239"/>
-      <c r="J7" s="241" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="251"/>
+      <c r="J7" s="253" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="240" t="s">
+      <c r="K7" s="252" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="29" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="239"/>
-      <c r="J8" s="241"/>
-      <c r="K8" s="240" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="251"/>
+      <c r="J8" s="253"/>
+      <c r="K8" s="252" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:14" s="29" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="169" t="s">
         <v>73</v>
       </c>
@@ -14486,7 +14504,7 @@
       <c r="I9" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="241"/>
+      <c r="J9" s="253"/>
       <c r="K9" s="173" t="s">
         <v>73</v>
       </c>
@@ -14496,25 +14514,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:14" s="29" customFormat="1">
-      <c r="A10" s="234" t="s">
+      <c r="A10" s="246" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="236"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="248"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
     </row>
     <row r="11" spans="1:14" s="38" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="66" t="s">
@@ -15100,7 +15118,7 @@
         <v>224</v>
       </c>
       <c r="F25" s="65" t="s">
-        <v>224</v>
+        <v>1023</v>
       </c>
       <c r="G25" s="180" t="s">
         <v>150</v>
@@ -15143,7 +15161,7 @@
         <v>229</v>
       </c>
       <c r="F26" s="65" t="s">
-        <v>229</v>
+        <v>1022</v>
       </c>
       <c r="G26" s="180" t="s">
         <v>150</v>
@@ -15186,7 +15204,7 @@
         <v>234</v>
       </c>
       <c r="F27" s="65" t="s">
-        <v>234</v>
+        <v>1021</v>
       </c>
       <c r="G27" s="180" t="s">
         <v>150</v>
@@ -15229,7 +15247,7 @@
         <v>238</v>
       </c>
       <c r="F28" s="65" t="s">
-        <v>238</v>
+        <v>1020</v>
       </c>
       <c r="G28" s="180" t="s">
         <v>150</v>
@@ -15272,7 +15290,7 @@
         <v>242</v>
       </c>
       <c r="F29" s="65" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
       <c r="G29" s="180" t="s">
         <v>150</v>
@@ -15315,7 +15333,7 @@
         <v>246</v>
       </c>
       <c r="F30" s="65" t="s">
-        <v>246</v>
+        <v>1019</v>
       </c>
       <c r="G30" s="180" t="s">
         <v>150</v>
@@ -15567,8 +15585,8 @@
   </sheetPr>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G21"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -15594,13 +15612,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="232" t="s">
+      <c r="B1" s="244" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -15614,13 +15632,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -15729,68 +15747,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="29" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="29" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:14" s="29" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -15800,7 +15818,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -15810,25 +15828,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:14" s="29" customFormat="1">
-      <c r="A10" s="235" t="s">
+      <c r="A10" s="247" t="s">
         <v>255</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="247"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
     </row>
     <row r="11" spans="1:14" s="38" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="66" t="s">
@@ -16446,13 +16464,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="K8:M8"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -16461,6 +16472,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="K8:M8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="G18:G21 G11:G16 K11:K16 K18:K21" xr:uid="{09908294-EEF3-4378-9490-F0CEFC2D3269}">
@@ -16481,7 +16499,7 @@
   </sheetPr>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:G21"/>
     </sheetView>
   </sheetViews>
@@ -16508,13 +16526,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -16528,13 +16546,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -16643,68 +16661,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:19" s="29" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="29" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:19" s="29" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -16714,7 +16732,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -16724,25 +16742,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:19" s="29" customFormat="1">
-      <c r="A10" s="234" t="s">
+      <c r="A10" s="246" t="s">
         <v>296</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="247"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
     </row>
     <row r="11" spans="1:19" s="38" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="68" t="s">
@@ -17411,8 +17429,8 @@
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21:K22"/>
+    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -17438,13 +17456,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -17458,13 +17476,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>349</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -17573,68 +17591,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -17644,7 +17662,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -17654,24 +17672,24 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:15" s="41" customFormat="1">
-      <c r="A10" s="242" t="s">
+      <c r="A10" s="254" t="s">
         <v>350</v>
       </c>
-      <c r="B10" s="242"/>
-      <c r="C10" s="242"/>
-      <c r="D10" s="242"/>
-      <c r="E10" s="242"/>
-      <c r="F10" s="242"/>
-      <c r="G10" s="242"/>
-      <c r="H10" s="242"/>
-      <c r="I10" s="242"/>
-      <c r="J10" s="242"/>
-      <c r="K10" s="242"/>
-      <c r="L10" s="242"/>
-      <c r="M10" s="242"/>
+      <c r="B10" s="254"/>
+      <c r="C10" s="254"/>
+      <c r="D10" s="254"/>
+      <c r="E10" s="254"/>
+      <c r="F10" s="254"/>
+      <c r="G10" s="254"/>
+      <c r="H10" s="254"/>
+      <c r="I10" s="254"/>
+      <c r="J10" s="254"/>
+      <c r="K10" s="254"/>
+      <c r="L10" s="254"/>
+      <c r="M10" s="254"/>
       <c r="N10" s="170"/>
       <c r="O10" s="76"/>
     </row>
@@ -18107,7 +18125,7 @@
       <c r="J21" s="123" t="s">
         <v>394</v>
       </c>
-      <c r="K21" s="261" t="s">
+      <c r="K21" s="201" t="s">
         <v>82</v>
       </c>
       <c r="L21" s="157" t="s">
@@ -18136,7 +18154,7 @@
         <v>398</v>
       </c>
       <c r="F22" s="123" t="s">
-        <v>398</v>
+        <v>1024</v>
       </c>
       <c r="G22" s="180" t="s">
         <v>150</v>
@@ -18626,13 +18644,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="J7:J9"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="A7:A9"/>
@@ -18641,6 +18652,13 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="J7:J9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" promptTitle="dfdf" sqref="K11:K18 G11:G18 G20:G33 K20:K33" xr:uid="{03194817-8C7E-405E-B5E0-431AACA99BF8}">
@@ -18661,8 +18679,8 @@
   </sheetPr>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -18688,13 +18706,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="231" t="s">
+      <c r="B1" s="243" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -18708,13 +18726,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>446</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -18823,68 +18841,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="245" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="257" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="169" t="s">
         <v>73</v>
       </c>
@@ -18894,7 +18912,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="169" t="s">
         <v>73</v>
       </c>
@@ -18904,25 +18922,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:15" s="41" customFormat="1">
-      <c r="A10" s="234" t="s">
+      <c r="A10" s="246" t="s">
         <v>447</v>
       </c>
-      <c r="B10" s="235"/>
-      <c r="C10" s="235"/>
-      <c r="D10" s="235"/>
-      <c r="E10" s="235"/>
-      <c r="F10" s="235"/>
-      <c r="G10" s="235"/>
-      <c r="H10" s="235"/>
-      <c r="I10" s="235"/>
-      <c r="J10" s="235"/>
-      <c r="K10" s="235"/>
-      <c r="L10" s="235"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="235"/>
+      <c r="B10" s="247"/>
+      <c r="C10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="247"/>
+      <c r="F10" s="247"/>
+      <c r="G10" s="247"/>
+      <c r="H10" s="247"/>
+      <c r="I10" s="247"/>
+      <c r="J10" s="247"/>
+      <c r="K10" s="247"/>
+      <c r="L10" s="247"/>
+      <c r="M10" s="247"/>
+      <c r="N10" s="247"/>
       <c r="O10" s="76"/>
     </row>
     <row r="11" spans="1:15" s="42" customFormat="1" ht="72" customHeight="1">
@@ -19094,10 +19112,10 @@
       <c r="N14" s="56"/>
     </row>
     <row r="15" spans="1:15" s="40" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A15" s="243" t="s">
+      <c r="A15" s="255" t="s">
         <v>469</v>
       </c>
-      <c r="B15" s="244"/>
+      <c r="B15" s="256"/>
       <c r="C15" s="88"/>
       <c r="D15" s="88"/>
       <c r="E15" s="88"/>
@@ -19518,72 +19536,72 @@
       <c r="F25" s="70" t="s">
         <v>517</v>
       </c>
-      <c r="G25" s="251" t="s">
-        <v>82</v>
-      </c>
-      <c r="H25" s="252">
+      <c r="G25" s="191" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="192">
         <v>45812</v>
       </c>
-      <c r="I25" s="253" t="s">
+      <c r="I25" s="193" t="s">
         <v>84</v>
       </c>
       <c r="J25" s="70" t="s">
         <v>517</v>
       </c>
-      <c r="K25" s="251" t="s">
-        <v>82</v>
-      </c>
-      <c r="L25" s="254" t="s">
+      <c r="K25" s="191" t="s">
+        <v>82</v>
+      </c>
+      <c r="L25" s="194" t="s">
         <v>453</v>
       </c>
-      <c r="M25" s="253" t="s">
+      <c r="M25" s="193" t="s">
         <v>84</v>
       </c>
       <c r="N25" s="133"/>
       <c r="O25" s="43"/>
     </row>
     <row r="26" spans="1:15" s="40" customFormat="1" ht="72" customHeight="1">
-      <c r="A26" s="256" t="s">
+      <c r="A26" s="196" t="s">
         <v>1014</v>
       </c>
-      <c r="B26" s="255" t="s">
+      <c r="B26" s="195" t="s">
         <v>1015</v>
       </c>
-      <c r="C26" s="255" t="s">
+      <c r="C26" s="195" t="s">
         <v>1016</v>
       </c>
-      <c r="D26" s="255" t="s">
+      <c r="D26" s="195" t="s">
         <v>487</v>
       </c>
-      <c r="E26" s="255" t="s">
+      <c r="E26" s="195" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F26" s="196" t="s">
         <v>1017</v>
       </c>
-      <c r="F26" s="256" t="s">
+      <c r="G26" s="202" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="197">
+        <v>45812</v>
+      </c>
+      <c r="I26" s="198" t="s">
+        <v>84</v>
+      </c>
+      <c r="J26" s="196" t="s">
+        <v>1017</v>
+      </c>
+      <c r="K26" s="202" t="s">
+        <v>150</v>
+      </c>
+      <c r="L26" s="199" t="s">
+        <v>453</v>
+      </c>
+      <c r="M26" s="198" t="s">
+        <v>84</v>
+      </c>
+      <c r="N26" s="200" t="s">
         <v>1018</v>
-      </c>
-      <c r="G26" s="262" t="s">
-        <v>150</v>
-      </c>
-      <c r="H26" s="257">
-        <v>45812</v>
-      </c>
-      <c r="I26" s="258" t="s">
-        <v>84</v>
-      </c>
-      <c r="J26" s="256" t="s">
-        <v>1018</v>
-      </c>
-      <c r="K26" s="262" t="s">
-        <v>150</v>
-      </c>
-      <c r="L26" s="259" t="s">
-        <v>453</v>
-      </c>
-      <c r="M26" s="258" t="s">
-        <v>84</v>
-      </c>
-      <c r="N26" s="260" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="40" customFormat="1" ht="72" customHeight="1">
@@ -19679,7 +19697,7 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11:G31"/>
     </sheetView>
   </sheetViews>
@@ -19706,13 +19724,13 @@
       <c r="A1" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="232" t="s">
+      <c r="B1" s="244" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="232"/>
-      <c r="D1" s="232"/>
-      <c r="E1" s="232"/>
-      <c r="F1" s="232"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="244"/>
+      <c r="E1" s="244"/>
+      <c r="F1" s="244"/>
       <c r="G1" s="45"/>
       <c r="H1" s="46"/>
       <c r="I1" s="47"/>
@@ -19726,13 +19744,13 @@
       <c r="A2" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="238" t="s">
+      <c r="B2" s="250" t="s">
         <v>518</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
       <c r="G2" s="45"/>
       <c r="H2" s="46"/>
       <c r="I2" s="47"/>
@@ -19841,68 +19859,68 @@
       <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:14" s="29" customFormat="1">
-      <c r="A7" s="233" t="s">
+      <c r="A7" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="233" t="s">
+      <c r="B7" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="233" t="s">
+      <c r="C7" s="245" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="233" t="s">
+      <c r="D7" s="245" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="233" t="s">
+      <c r="E7" s="245" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="233" t="s">
+      <c r="F7" s="245" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="233" t="s">
+      <c r="G7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="233"/>
-      <c r="I7" s="233"/>
-      <c r="J7" s="228" t="s">
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="240" t="s">
         <v>519</v>
       </c>
-      <c r="K7" s="233" t="s">
+      <c r="K7" s="245" t="s">
         <v>71</v>
       </c>
-      <c r="L7" s="233"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233" t="s">
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="29" customFormat="1">
-      <c r="A8" s="233"/>
-      <c r="B8" s="233"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
-      <c r="G8" s="233" t="s">
+      <c r="A8" s="245"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="245"/>
+      <c r="D8" s="245"/>
+      <c r="E8" s="245"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="233"/>
-      <c r="I8" s="233"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="233" t="s">
+      <c r="H8" s="245"/>
+      <c r="I8" s="245"/>
+      <c r="J8" s="241"/>
+      <c r="K8" s="245" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="233"/>
-      <c r="N8" s="233"/>
+      <c r="L8" s="245"/>
+      <c r="M8" s="245"/>
+      <c r="N8" s="245"/>
     </row>
     <row r="9" spans="1:14" s="29" customFormat="1">
-      <c r="A9" s="233"/>
-      <c r="B9" s="233"/>
-      <c r="C9" s="233"/>
-      <c r="D9" s="233"/>
-      <c r="E9" s="233"/>
-      <c r="F9" s="233"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
       <c r="G9" s="174" t="s">
         <v>73</v>
       </c>
@@ -19912,7 +19930,7 @@
       <c r="I9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="230"/>
+      <c r="J9" s="242"/>
       <c r="K9" s="174" t="s">
         <v>73</v>
       </c>
@@ -19922,25 +19940,25 @@
       <c r="M9" s="169" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="233"/>
+      <c r="N9" s="245"/>
     </row>
     <row r="10" spans="1:14" s="29" customFormat="1">
-      <c r="A10" s="234" t="s">
+      <c r="A10" s="246" t="s">
         <v>520</v>
       </c>
-      <c r="B10" s="234"/>
-      <c r="C10" s="234"/>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="234"/>
-      <c r="H10" s="234"/>
-      <c r="I10" s="234"/>
-      <c r="J10" s="234"/>
-      <c r="K10" s="234"/>
-      <c r="L10" s="234"/>
-      <c r="M10" s="234"/>
-      <c r="N10" s="234"/>
+      <c r="B10" s="246"/>
+      <c r="C10" s="246"/>
+      <c r="D10" s="246"/>
+      <c r="E10" s="246"/>
+      <c r="F10" s="246"/>
+      <c r="G10" s="246"/>
+      <c r="H10" s="246"/>
+      <c r="I10" s="246"/>
+      <c r="J10" s="246"/>
+      <c r="K10" s="246"/>
+      <c r="L10" s="246"/>
+      <c r="M10" s="246"/>
+      <c r="N10" s="246"/>
     </row>
     <row r="11" spans="1:14" s="38" customFormat="1" ht="72" customHeight="1">
       <c r="A11" s="68" t="s">
@@ -20363,10 +20381,10 @@
       <c r="N20" s="55"/>
     </row>
     <row r="21" spans="1:14" s="39" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A21" s="225" t="s">
+      <c r="A21" s="237" t="s">
         <v>568</v>
       </c>
-      <c r="B21" s="226"/>
+      <c r="B21" s="238"/>
       <c r="C21" s="88"/>
       <c r="D21" s="88"/>
       <c r="E21" s="88"/>

</xml_diff>